<commit_message>
updated script and  indicator name change, and added ranking instructions
</commit_message>
<xml_diff>
--- a/input/INDICATORS_TO_RANK.xlsx
+++ b/input/INDICATORS_TO_RANK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="15180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="580" yWindow="1220" windowWidth="28160" windowHeight="15180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="424">
   <si>
     <t>N_info_source_who</t>
   </si>
@@ -1035,7 +1035,271 @@
     <t>F_mortality_increase_why_malaria_fever</t>
   </si>
   <si>
+    <t>D2_idp_time_arrive</t>
+  </si>
+  <si>
+    <t>D2_idp_source_lga</t>
+  </si>
+  <si>
+    <t>D2_idp_source_ward</t>
+  </si>
+  <si>
+    <t>D_D2_idp_time_arrive_1_month</t>
+  </si>
+  <si>
+    <t>D_D2_idp_time_arrive_1_year</t>
+  </si>
+  <si>
+    <t>D_D2_idp_time_arrive_3_months</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_bama</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_dikwa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_guzamala</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_gwoza</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_kala_balge</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_kukawa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_lga_marte</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_afuye</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_ashigashiya</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_baga</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_bita_izge</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_boboshe</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_chikide</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_daima</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_darajamal</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_gajibo</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_gava_agapalawa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_guduf_a_b</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_gudumbali_west</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_hambagda</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_jilbe</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_kala</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_kirawa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_kirenowa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_kuranabasa</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_m._maja</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_mairari</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_moduri</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_ngoshe</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_ngudoram</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_other</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_pulka_bokko</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_rann</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_soye</t>
+  </si>
+  <si>
+    <t>D_D2_idp_source_ward_wala_warabe</t>
+  </si>
+  <si>
+    <t>D_D3_returnee_time_arrived_1_month</t>
+  </si>
+  <si>
+    <t>D_D3_returnee_time_arrived_1_year</t>
+  </si>
+  <si>
+    <t>D_D3_returnee_time_arrived_3_months</t>
+  </si>
+  <si>
+    <t>D_D3_returnee_time_arrived_4_6_months</t>
+  </si>
+  <si>
+    <t>D_D3_returnee_time_arrived_7_12_months</t>
+  </si>
+  <si>
+    <t>Bama</t>
+  </si>
+  <si>
+    <t>Dikwa</t>
+  </si>
+  <si>
+    <t>Guzamala</t>
+  </si>
+  <si>
+    <t>Gwoza</t>
+  </si>
+  <si>
+    <t>Kala Balge</t>
+  </si>
+  <si>
+    <t>Kukawa</t>
+  </si>
+  <si>
+    <t>Marte</t>
+  </si>
+  <si>
+    <t>Afuye</t>
+  </si>
+  <si>
+    <t>Ashigashiya</t>
+  </si>
+  <si>
+    <t>Baga</t>
+  </si>
+  <si>
+    <t>Bita Izge</t>
+  </si>
+  <si>
+    <t>Boboshe</t>
+  </si>
+  <si>
+    <t>Chikide</t>
+  </si>
+  <si>
+    <t>Daima</t>
+  </si>
+  <si>
+    <t>Darajamal</t>
+  </si>
+  <si>
+    <t>Gajibo</t>
+  </si>
+  <si>
+    <t>Gava Agapalawa</t>
+  </si>
+  <si>
+    <t>Guduf</t>
+  </si>
+  <si>
+    <t>Gudumbali West</t>
+  </si>
+  <si>
+    <t>Hambagda</t>
+  </si>
+  <si>
+    <t>Jilbe</t>
+  </si>
+  <si>
+    <t>Kala</t>
+  </si>
+  <si>
+    <t>Kirawa</t>
+  </si>
+  <si>
+    <t>Kirenowa</t>
+  </si>
+  <si>
+    <t>Kuranabasa</t>
+  </si>
+  <si>
+    <t>M. Maya</t>
+  </si>
+  <si>
+    <t>Mairari</t>
+  </si>
+  <si>
+    <t>Moduri</t>
+  </si>
+  <si>
+    <t>Ngoshe</t>
+  </si>
+  <si>
+    <t>Ngudoram</t>
+  </si>
+  <si>
+    <t>Pulka Bokko</t>
+  </si>
+  <si>
+    <t>Rann</t>
+  </si>
+  <si>
+    <t>Soye</t>
+  </si>
+  <si>
+    <t>Wala Warabe</t>
+  </si>
+  <si>
+    <t>1 Month</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>4-6 Months</t>
+  </si>
+  <si>
+    <t>7-12 Months</t>
+  </si>
+  <si>
     <t>F_mortality_increase_why_other</t>
+  </si>
+  <si>
+    <t>D3_returnee_time_arrived</t>
+  </si>
+  <si>
+    <t>D_D2_idp_time_arrive_7_12_months</t>
+  </si>
+  <si>
+    <t>D_D2_idp_time_arrive_4_6_months</t>
   </si>
 </sst>
 </file>
@@ -1079,13 +1343,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1363,9 +1630,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1374,151 +1643,171 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1529,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B193"/>
+  <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="B237" sqref="B237:B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,7 +2078,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>90</v>
       </c>
@@ -2445,7 +2734,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>217</v>
       </c>
@@ -3078,11 +3367,376 @@
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>335</v>
+      <c r="A193" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="B193" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B194" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B195" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B196" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B197" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B198" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B199" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B200" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B201" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B202" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B203" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B204" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B205" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B206" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B207" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B208" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B209" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B210" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B211" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B212" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B213" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B214" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B215" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B216" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B217" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B218" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B219" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B220" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B221" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B222" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B223" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B224" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A225" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B225" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B226" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A227" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B227" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A228" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B228" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A229" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B229" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B230" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A231" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B231" t="s">
+        <v>414</v>
+      </c>
+      <c r="E231" s="4"/>
+      <c r="F231" s="4"/>
+      <c r="G231" s="4"/>
+      <c r="H231" s="4"/>
+      <c r="I231" s="4"/>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A232" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B232" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A233" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B233" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A234" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B234" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A235" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B235" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A236" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B236" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>422</v>
+      </c>
+      <c r="B237" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>423</v>
+      </c>
+      <c r="B238" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>